<commit_message>
Added the files that will be the English version of Shan Hai
</commit_message>
<xml_diff>
--- a/中文/空白人物卡.xlsx
+++ b/中文/空白人物卡.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitStuff\Tao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitStuff\Tao\中文\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981F09E5-892D-43A5-994C-61E422DB2B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898D5FD0-3E03-4E56-9BEA-7D9CF1252545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="0" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -267,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,20 +279,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -578,7 +574,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="B7" sqref="B7:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -594,22 +590,22 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" t="s">
         <v>19</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="8">
         <f>(E2/F2)%</f>
         <v>0.01</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -642,13 +638,13 @@
       <c r="F3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="8">
         <f>(E4/F4)%</f>
         <v>0.01</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -679,21 +675,21 @@
       <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6">
-        <f>10+IF(G7="重甲",0,E15)+H7</f>
+        <f>10+IF(G7="重甲",0,E15)+H7+IF(H9&gt;0,G9,0)</f>
         <v>12</v>
       </c>
       <c r="F6" t="s">
@@ -707,13 +703,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
       <c r="G7" t="s">
         <v>48</v>
       </c>
@@ -722,11 +718,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
       <c r="F8" t="s">
         <v>20</v>
       </c>
@@ -738,18 +734,18 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
       <c r="F10" t="s">
         <v>46</v>
       </c>
@@ -761,18 +757,18 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="F12" t="s">
         <v>47</v>
       </c>
@@ -818,10 +814,10 @@
         <f>D14-5</f>
         <v>2</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -841,14 +837,14 @@
         <f t="shared" ref="E15:E19" si="1">D15-5</f>
         <v>1</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -868,10 +864,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -894,13 +890,13 @@
       <c r="F17" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -920,9 +916,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -942,20 +937,18 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="9"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -964,145 +957,134 @@
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="9"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="9"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>3</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>4</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>5</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>6</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>7</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>8</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>9</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>10</v>
       </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -1116,80 +1098,64 @@
         <v>33</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1198,21 +1164,10 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B7:E11"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G3:J3"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="A7:A11"/>
@@ -1227,10 +1182,21 @@
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B7:E11"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G4">

</xml_diff>